<commit_message>
fix carriage return issues in declarations text
</commit_message>
<xml_diff>
--- a/docs/data/local_authority_climate_emergency_declarations/0/local_authority_climate_emergency_declarations.xlsx
+++ b/docs/data/local_authority_climate_emergency_declarations/0/local_authority_climate_emergency_declarations.xlsx
@@ -46,7 +46,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.1</t>
   </si>
   <si>
     <t>Contributors</t>
@@ -1831,8 +1831,7 @@
     <t>Kettering Borough Council (defunct council)</t>
   </si>
   <si>
-    <t>King's Lynn and West Norfolk Borough
-Council</t>
+    <t>King's Lynn and West Norfolk BoroughCouncil</t>
   </si>
   <si>
     <t>Kirklees Council</t>
@@ -2252,8 +2251,7 @@
     <t>Somerset West and Taunton Council</t>
   </si>
   <si>
-    <t>South Buckinghamshire District
-Council</t>
+    <t>South Buckinghamshire DistrictCouncil</t>
   </si>
   <si>
     <t>South Cambridgeshire District Council</t>
@@ -3207,8 +3205,7 @@
     <t>Climate Change motion (not Climate Emergency)</t>
   </si>
   <si>
-    <t>Link to article
-Link to minutes</t>
+    <t>Link to articleLink to minutes</t>
   </si>
   <si>
     <t>Link (ignore wrong date in title of the document)</t>
@@ -3352,8 +3349,7 @@
     <t>Yes - Ecological Emergency (separate - Oct 2020)</t>
   </si>
   <si>
-    <t>No - but it is one of the guiding principles for the Action Plan
-A motion to declare an ecological emergency was withdrawn in December 2020</t>
+    <t>No - but it is one of the guiding principles for the Action PlanA motion to declare an ecological emergency was withdrawn in December 2020</t>
   </si>
   <si>
     <t>Yes - "Climate Change and Biodiversity Emergency"</t>
@@ -3374,14 +3370,13 @@
     <t>Yes - 'Climate and Ecological Emergency</t>
   </si>
   <si>
-    <t>Yes, "We are recognising a biodiversity or ecological crisis as_x000D_ implicit within the declaration of ‘climate emergency’."_x000D_</t>
+    <t>Yes, "We are recognising a biodiversity or ecological crisis as implicit within the declaration of ‘climate emergency’."</t>
   </si>
   <si>
     <t>Yes - climate and ecological emergency</t>
   </si>
   <si>
-    <t xml:space="preserve">Unsure - 'recognised that climate change is an ecological emergency'
-</t>
+    <t>Unsure - 'recognised that climate change is an ecological emergency'</t>
   </si>
   <si>
     <t>Yes (climate and biodiversity declaration)</t>
@@ -3414,7 +3409,7 @@
     <t>Yes - "Environmental and Climate Change"</t>
   </si>
   <si>
-    <t>Yes "promoting biodiversity;"_x000D_</t>
+    <t>Yes "promoting biodiversity;"</t>
   </si>
   <si>
     <t>Yes (Environment)</t>
@@ -3429,8 +3424,7 @@
     <t>Yes "strategic actions needed to address the environment and climate emergency"</t>
   </si>
   <si>
-    <t>Yes in preamble "loss of biodiversity including insects and vital food crop pollinators.
-"</t>
+    <t>Yes in preamble "loss of biodiversity including insects and vital food crop pollinators."</t>
   </si>
   <si>
     <t>No (deleted points 2-6 of motion that did reference biodiversity)</t>
@@ -3439,14 +3433,13 @@
     <t>Declared</t>
   </si>
   <si>
-    <t>Yes "protecting biodiversity"
-"Partnership; managing and protecting our County wildlife sites and their _x000D_biodiversity"</t>
+    <t>Yes "protecting biodiversity""Partnership; managing and protecting our County wildlife sites and their biodiversity"</t>
   </si>
   <si>
     <t>Yes - "Council Scrutiny Panels consider the impact of climate change and the environment when reviewing Council policies and strategies"</t>
   </si>
   <si>
-    <t>Declared. Also "Establish a baseline for Chelmsford’s ecological status and monitor progress year on year" _x000D_</t>
+    <t xml:space="preserve">Declared. Also "Establish a baseline for Chelmsford’s ecological status and monitor progress year on year" </t>
   </si>
   <si>
     <t>No (but useful info)</t>
@@ -3455,7 +3448,7 @@
     <t>Yes "loss of biodiversity including insects and... pollinators"</t>
   </si>
   <si>
-    <t>Yes "Commission an environmental audit which identifies pollution hotspots, wildlife biodiversity... aim to identify areas of improvement across the borough._x000D_ _x000D_</t>
+    <t xml:space="preserve">Yes "Commission an environmental audit which identifies pollution hotspots, wildlife biodiversity... aim to identify areas of improvement across the borough. </t>
   </si>
   <si>
     <t>Yes - "man made ecological crisis"; "set commitment to improve biodiversity"</t>
@@ -3482,8 +3475,7 @@
     <t>No - later added to terms of reference of CE group</t>
   </si>
   <si>
-    <t>Declared &amp; "Resolves to put sustainability, biodiversity and carbon reduction at the heart of_x000D_
-this Council’s agenda"</t>
+    <t>Declared &amp; "Resolves to put sustainability, biodiversity and carbon reduction at the heart ofthis Council’s agenda"</t>
   </si>
   <si>
     <t>Declared later - Nov 2019</t>
@@ -3492,8 +3484,7 @@
     <t>Yes - Staff report on CE "in report highlights biodiversity and actions"</t>
   </si>
   <si>
-    <t>Yes "recognise the importance of our biodiversity and natural environment."
-"will incorporate actions on loss of biodiversity and our natural environment;"_x000D__x000D_</t>
+    <t>Yes "recognise the importance of our biodiversity and natural environment.""will incorporate actions on loss of biodiversity and our natural environment;"</t>
   </si>
   <si>
     <t>Yes "recognised the serious and accelerating environmental faced by climate change and declared a climate emergency"</t>
@@ -3505,14 +3496,13 @@
     <t>Yes "Plan... to protect and enhance biodiversity"</t>
   </si>
   <si>
-    <t>Yes "Set up an Environmental and Climate Forum"
-"very best measures into the Local Plan to minimise any negative impact on the environment"</t>
+    <t>Yes "Set up an Environmental and Climate Forum""very best measures into the Local Plan to minimise any negative impact on the environment"</t>
   </si>
   <si>
     <t>No but Ecological emergency recognised as part of plan</t>
   </si>
   <si>
-    <t>Yes "Carbon off-setting measures- for example using nature to take carbon..." _x000D_</t>
+    <t xml:space="preserve">Yes "Carbon off-setting measures- for example using nature to take carbon..." </t>
   </si>
   <si>
     <t>No but referenced later</t>
@@ -3524,16 +3514,16 @@
     <t>Yes "Seek to increase the number and size of land designated as nature reserves and improve and create habitats to support insect life including bees"</t>
   </si>
   <si>
-    <t>Yes "Exeter City Council recognises the connected biodiversity crisis"_x000D_</t>
-  </si>
-  <si>
-    <t>Yes "noted the focus on increasing Biodiversity"_x000D_</t>
+    <t>Yes "Exeter City Council recognises the connected biodiversity crisis"</t>
+  </si>
+  <si>
+    <t>Yes "noted the focus on increasing Biodiversity"</t>
   </si>
   <si>
     <t>No - but later referred to as declared</t>
   </si>
   <si>
-    <t>Yes - preamble "species loss and extinction"_x000D_</t>
+    <t>Yes - preamble "species loss and extinction"</t>
   </si>
   <si>
     <t xml:space="preserve">Yes "Gwynedd's landscape presents many opportunities for... biodiversity regeneration" </t>
@@ -3551,7 +3541,7 @@
     <t>Yes - "Work to mitigate the biodiversity crisis in its actions across the Borough"</t>
   </si>
   <si>
-    <t>Yes - "and biodiversity loss and we support action to tackle these matters."_x000D_</t>
+    <t>Yes - "and biodiversity loss and we support action to tackle these matters."</t>
   </si>
   <si>
     <t>Not in CE declaration but referenced after</t>
@@ -3578,18 +3568,16 @@
     <t>Yes in preamble "danger to people and biodiversity from climate change."</t>
   </si>
   <si>
-    <t>No
-but later added to plan objectives</t>
-  </si>
-  <si>
-    <t>Later noted 19/03/20 to add on to CE 
-"(3)          the wider ecological implications of the human-induced changes that were occurring to our climate be noted;"</t>
+    <t>Nobut later added to plan objectives</t>
+  </si>
+  <si>
+    <t>Later noted 19/03/20 to add on to CE "(3)          the wider ecological implications of the human-induced changes that were occurring to our climate be noted;"</t>
   </si>
   <si>
     <t>Yes "recognise... changing climate will have severe and enduring... environmental implications"</t>
   </si>
   <si>
-    <t>Yes "9. Improve biodiversity and carbon storage (e.g. tree planting)_x000D_"</t>
+    <t>Yes "9. Improve biodiversity and carbon storage (e.g. tree planting)"</t>
   </si>
   <si>
     <t>Yes "Protecting Southwark’s biodiversity"</t>
@@ -3610,18 +3598,16 @@
     <t>Yes "This council is significantly concerned that the environmental crises must be a priority."</t>
   </si>
   <si>
-    <t>Yes "Request that Council Scrutiny Panels consider the impact of climate change and the _x000D_environment when reviewing Council policies and strategies;_x000D_"</t>
+    <t>Yes "Request that Council Scrutiny Panels consider the impact of climate change and the environment when reviewing Council policies and strategies;"</t>
   </si>
   <si>
     <t>Yes "clean air and biodiversity are key to a sustainable city"</t>
   </si>
   <si>
-    <t>Yes "increasingly erratic climate and biodiversity loss."
-And action point "make a positively beneficial impact on the _x000D_environment and biodiversity in the District."_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes "We have a strong track record in our sustainability and environment stewardship. We have engaged in climate change actions for many years and, through policies and activities, have made the district more resilient, reduced carbon emissions, created space for nature, and provided the infrastructure to enable others to make choices that reduce emissions. Going forward, we will be taking more actions in every area of our day-to-day activities, in our operations, our civic buildings and depots, improving our natural environment to support nature recovery, as well as gaining a better understanding and measurement of what the issues are and what our actions are achieving.
-A Sustainability Advisory Member Panel will now set actions to address the climate and nature emergency and will present a report to full Council in February 2022. </t>
+    <t>Yes "increasingly erratic climate and biodiversity loss."And action point "make a positively beneficial impact on the environment and biodiversity in the District."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes "We have a strong track record in our sustainability and environment stewardship. We have engaged in climate change actions for many years and, through policies and activities, have made the district more resilient, reduced carbon emissions, created space for nature, and provided the infrastructure to enable others to make choices that reduce emissions. Going forward, we will be taking more actions in every area of our day-to-day activities, in our operations, our civic buildings and depots, improving our natural environment to support nature recovery, as well as gaining a better understanding and measurement of what the issues are and what our actions are achieving.A Sustainability Advisory Member Panel will now set actions to address the climate and nature emergency and will present a report to full Council in February 2022. </t>
   </si>
   <si>
     <t>Yes, "extinctions of plant, insect and animal species"</t>
@@ -3639,7 +3625,7 @@
     <t>Yes on Sept 24th 2019.</t>
   </si>
   <si>
-    <t>Yes "harmful effects climate change has on... natural habitats and eco-systems."_x000D_</t>
+    <t>Yes "harmful effects climate change has on... natural habitats and eco-systems."</t>
   </si>
   <si>
     <t>Yes - references "climate and environmental emergency" in preamble</t>
@@ -3648,8 +3634,7 @@
     <t>Yes - "the health of ecosystems on which we depend is deteriorating more rapidly"</t>
   </si>
   <si>
-    <t>No
-Although will be addressed in Local Plan review</t>
+    <t>NoAlthough will be addressed in Local Plan review</t>
   </si>
   <si>
     <t>Reference in minutes rather than motion</t>
@@ -3667,8 +3652,7 @@
     <t>Yes, "problems of climate change, air pollution and reduction of species &amp; biodiversity need to be treated together"</t>
   </si>
   <si>
-    <t>Yes in CE declaration "greater loss of species and habitats, changing ecosystems"
-Later declared</t>
+    <t>Yes in CE declaration "greater loss of species and habitats, changing ecosystems"Later declared</t>
   </si>
   <si>
     <t>Not in CE declaration but declared separately</t>
@@ -3680,16 +3664,13 @@
     <t>Yes "changes in ecosystems"</t>
   </si>
   <si>
-    <t>Included in declaration - 'business as usual not an option in the face of the climate and biodiversity emergency'.
-Theme in Action Plan</t>
-  </si>
-  <si>
-    <t>Declared 
-Also included in action plan. And have separate biodiversity action plan (2016)</t>
-  </si>
-  <si>
-    <t>Yes "duty to limit the negative impacts of... biodiversity loss" 
-Also mentioned in Climate Action Plan</t>
+    <t>Included in declaration - 'business as usual not an option in the face of the climate and biodiversity emergency'.Theme in Action Plan</t>
+  </si>
+  <si>
+    <t>Declared Also included in action plan. And have separate biodiversity action plan (2016)</t>
+  </si>
+  <si>
+    <t>Yes "duty to limit the negative impacts of... biodiversity loss" Also mentioned in Climate Action Plan</t>
   </si>
   <si>
     <t>Yes - not in declaration but state they declared "environment and climate emergency" on plans normal page</t>
@@ -3707,19 +3688,16 @@
     <t>Yes "catastrophic consequences for humans and the natural world."</t>
   </si>
   <si>
-    <t>Declared
-Also in climate action strategy</t>
-  </si>
-  <si>
-    <t>Declared
-Also in plan - actions here</t>
+    <t>DeclaredAlso in climate action strategy</t>
+  </si>
+  <si>
+    <t>DeclaredAlso in plan - actions here</t>
   </si>
   <si>
     <t>No but mentions creation of new woodland in CE declaration.</t>
   </si>
   <si>
-    <t>Declared
-Also a section in climate plan</t>
+    <t>DeclaredAlso a section in climate plan</t>
   </si>
   <si>
     <t xml:space="preserve">Yes - separate. </t>
@@ -3728,15 +3706,13 @@
     <t>Not in declaration</t>
   </si>
   <si>
-    <t>Yes, "protect, maintain and enhance our natural environment" in climate emergency declaration_x000D_
-Climate Strategy is here. Mentions biodiversity with some actions listed.</t>
+    <t>Yes, "protect, maintain and enhance our natural environment" in climate emergency declarationClimate Strategy is here. Mentions biodiversity with some actions listed.</t>
   </si>
   <si>
     <t>Yes, policy statement here</t>
   </si>
   <si>
-    <t>Yes in declaration 'recognise that there is a Climate and Ecological Emergency; and that the Council formally declares a Climate Emergency'
-has separate Biodiversity Action Plan called Natural Woking (2016)</t>
+    <t>Yes in declaration 'recognise that there is a Climate and Ecological Emergency; and that the Council formally declares a Climate Emergency'has separate Biodiversity Action Plan called Natural Woking (2016)</t>
   </si>
   <si>
     <t>YES</t>
@@ -3772,10 +3748,7 @@
     <t>Yes - call on Lancashire County Council and Westminster</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes - Welsh and UK governments and
-"ask that Welsh and UK Government call on World Leaders to acknowledge the overwhelming scientific evidence that Climate Change has been created by human 
-activity" 
-</t>
+    <t xml:space="preserve">Yes - Welsh and UK governments and"ask that Welsh and UK Government call on World Leaders to acknowledge the overwhelming scientific evidence that Climate Change has been created by human activity" </t>
   </si>
   <si>
     <t>Yes "and local MPS"</t>
@@ -3784,7 +3757,7 @@
     <t>Yes - Welsh and UK governments</t>
   </si>
   <si>
-    <t>Yes "write to... SoS for Business, Energy &amp; Industrial Strategy; Transport; Environment, Food and Rural Affairs; and Housing, Communities and Local Government"_x000D_</t>
+    <t>Yes "write to... SoS for Business, Energy &amp; Industrial Strategy; Transport; Environment, Food and Rural Affairs; and Housing, Communities and Local Government"</t>
   </si>
   <si>
     <t>Yes "make representations to Welsh and UK"</t>
@@ -3811,8 +3784,7 @@
     <t>Yes "lobby, support and work with all relevant agencies"</t>
   </si>
   <si>
-    <t>Yes "work with"
-Detail letters and resposes from DFT here</t>
+    <t>Yes "work with"Detail letters and resposes from DFT here</t>
   </si>
   <si>
     <t>Yes "writing to... request funding"</t>
@@ -3842,7 +3814,7 @@
     <t xml:space="preserve">Yes </t>
   </si>
   <si>
-    <t>Yes "seek an urgent meeting with the Secretary of State for the Environment... to present Liverpool’s concerns and ideas raised by the dedicated Climate Change Council"_x000D__x000D_</t>
+    <t>Yes "seek an urgent meeting with the Secretary of State for the Environment... to present Liverpool’s concerns and ideas raised by the dedicated Climate Change Council"</t>
   </si>
   <si>
     <t>Yes (in their non declaration)</t>
@@ -3866,8 +3838,7 @@
     <t>Yes "urgent representations"</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes "write to Chancellor of Exchequer... funding be made available"
-Noted they wrote </t>
+    <t xml:space="preserve">Yes "write to Chancellor of Exchequer... funding be made available"Noted they wrote </t>
   </si>
   <si>
     <t>No - inform MPs, government of the commitment</t>
@@ -3921,11 +3892,10 @@
     <t>None (Vision document says target will be set with strategy)</t>
   </si>
   <si>
-    <t>2045 "Work with others across the region to ensure that Aberdeenshire reaches Net _x000D_Zero by 2045"</t>
-  </si>
-  <si>
-    <t>2050
-Also confirmed as 2050 from this Scatter report</t>
+    <t>2045 "Work with others across the region to ensure that Aberdeenshire reaches Net Zero by 2045"</t>
+  </si>
+  <si>
+    <t>2050Also confirmed as 2050 from this Scatter report</t>
   </si>
   <si>
     <t>2030 (confirmed)</t>
@@ -4033,8 +4003,7 @@
     <t>2045 (2030 is only for a singular town - Grangemouth</t>
   </si>
   <si>
-    <t xml:space="preserve">2050 (and deliver a carbon neutral county by 2050)
-</t>
+    <t>2050 (and deliver a carbon neutral county by 2050)</t>
   </si>
   <si>
     <t>2030 (prepare for the borough to be carbon neutral)</t>
@@ -4055,14 +4024,13 @@
     <t>None (2030 - "promoting community, public, business and other council partnerships to achieve this carbon neutral 2030")</t>
   </si>
   <si>
-    <t>2030 "entire area zero carbon within the same timescale._x000D_"</t>
+    <t>2030 "entire area zero carbon within the same timescale."</t>
   </si>
   <si>
     <t>2030 "District Zero Carbon within the same timescale;"</t>
   </si>
   <si>
-    <t xml:space="preserve">2030 "Agreement goal, our ambition is for Leicester to become ‘carbon neutral’ by 2030 or sooner. This means reducing the city’s and the council’s CO2 emissions to nearly zero
-</t>
+    <t>2030 "Agreement goal, our ambition is for Leicester to become ‘carbon neutral’ by 2030 or sooner. This means reducing the city’s and the council’s CO2 emissions to nearly zero</t>
   </si>
   <si>
     <t>None - Unsure as in CE declaration it states: "Support the Government’s target of Net Zero Carbon Emission by 2050"</t>
@@ -4134,12 +4102,10 @@
     <t>Council - abolished</t>
   </si>
   <si>
-    <t>2030
-Not sure if this is the date given councils plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2028 (Support and work with all partners in the City towards making the city zero carbon within the same timescale)
-</t>
+    <t>2030Not sure if this is the date given councils plan</t>
+  </si>
+  <si>
+    <t>2028 (Support and work with all partners in the City towards making the city zero carbon within the same timescale)</t>
   </si>
   <si>
     <t>*"The council supports measures to address the climate emergency"</t>
@@ -7051,7 +7017,7 @@
     <col min="6" max="6" width="132.7109375" customWidth="1"/>
     <col min="7" max="7" width="54.7109375" customWidth="1"/>
     <col min="8" max="8" width="220.7109375" customWidth="1"/>
-    <col min="9" max="9" width="849.7109375" customWidth="1"/>
+    <col min="9" max="9" width="847.7109375" customWidth="1"/>
     <col min="10" max="10" width="318.7109375" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="202.7109375" customWidth="1"/>

</xml_diff>